<commit_message>
Update script to include query for authors
</commit_message>
<xml_diff>
--- a/cumulative-totals.xlsx
+++ b/cumulative-totals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t xml:space="preserve">week</t>
   </si>
@@ -35,6 +35,15 @@
   </si>
   <si>
     <t xml:space="preserve">comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contributions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">authors</t>
   </si>
 </sst>
 </file>
@@ -203,7 +212,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -293,263 +302,263 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$G$2:$G$42</c:f>
+              <c:f>Sheet1!$K$2:$K$42</c:f>
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>11/09/15 09:15 AM</c:v>
+                  <c:v>11/02/15 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12/09/15 09:15 AM</c:v>
+                  <c:v>12/02/15 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>01/09/16 09:15 AM</c:v>
+                  <c:v>01/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>02/09/16 09:15 AM</c:v>
+                  <c:v>02/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>03/09/16 09:15 AM</c:v>
+                  <c:v>03/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>04/09/16 09:15 AM</c:v>
+                  <c:v>04/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>05/09/16 09:15 AM</c:v>
+                  <c:v>05/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>06/09/16 09:15 AM</c:v>
+                  <c:v>06/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>07/09/16 09:15 AM</c:v>
+                  <c:v>07/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>08/09/16 09:15 AM</c:v>
+                  <c:v>08/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>09/09/16 09:15 AM</c:v>
+                  <c:v>09/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10/09/16 09:15 AM</c:v>
+                  <c:v>10/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11/09/16 09:15 AM</c:v>
+                  <c:v>11/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12/09/16 09:15 AM</c:v>
+                  <c:v>12/02/16 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>01/09/17 09:15 AM</c:v>
+                  <c:v>01/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>02/09/17 09:15 AM</c:v>
+                  <c:v>02/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>03/09/17 09:15 AM</c:v>
+                  <c:v>03/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>04/09/17 09:15 AM</c:v>
+                  <c:v>04/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>05/09/17 09:15 AM</c:v>
+                  <c:v>05/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>06/09/17 09:15 AM</c:v>
+                  <c:v>06/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>07/09/17 09:15 AM</c:v>
+                  <c:v>07/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>08/09/17 09:15 AM</c:v>
+                  <c:v>08/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>09/09/17 09:15 AM</c:v>
+                  <c:v>09/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10/09/17 09:15 AM</c:v>
+                  <c:v>10/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11/09/17 09:15 AM</c:v>
+                  <c:v>11/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12/09/17 09:15 AM</c:v>
+                  <c:v>12/02/17 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>01/09/18 09:15 AM</c:v>
+                  <c:v>01/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>02/09/18 09:15 AM</c:v>
+                  <c:v>02/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>03/09/18 09:15 AM</c:v>
+                  <c:v>03/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>04/09/18 09:15 AM</c:v>
+                  <c:v>04/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>05/09/18 09:15 AM</c:v>
+                  <c:v>05/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>06/09/18 09:15 AM</c:v>
+                  <c:v>06/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>07/09/18 09:15 AM</c:v>
+                  <c:v>07/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>08/09/18 09:15 AM</c:v>
+                  <c:v>08/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>09/09/18 09:15 AM</c:v>
+                  <c:v>09/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>10/09/18 09:15 AM</c:v>
+                  <c:v>10/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11/09/18 09:15 AM</c:v>
+                  <c:v>11/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>12/09/18 09:15 AM</c:v>
+                  <c:v>12/02/18 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>01/09/19 09:15 AM</c:v>
+                  <c:v>01/02/19 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>02/09/19 09:15 AM</c:v>
+                  <c:v>02/02/19 05:27 PM</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>03/09/19 09:15 AM</c:v>
+                  <c:v>03/02/19 05:27 PM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$42</c:f>
+              <c:f>Sheet1!$M$2:$M$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>37</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>62</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>106</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>143</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>206</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>309</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>382</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>447</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>551</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>561</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>623</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>627</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>629</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>630</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>634</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>662</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>695</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>752</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>836</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>923</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>966</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>996</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1069</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1099</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1159</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1199</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1328</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1405</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1473</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1532</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1610</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1795</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1897</c:v>
+                  <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1991</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2008</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -564,11 +573,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="56956685"/>
-        <c:axId val="7413877"/>
+        <c:axId val="36760240"/>
+        <c:axId val="47225303"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56956685"/>
+        <c:axId val="36760240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,14 +608,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7413877"/>
+        <c:crossAx val="47225303"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7413877"/>
+        <c:axId val="47225303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,10 +646,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56956685"/>
+        <c:crossAx val="36760240"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="500"/>
+        <c:majorUnit val="50"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -703,10 +712,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -744,6 +753,21 @@
       <c r="H1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -770,6 +794,21 @@
       <c r="H2" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="I2" s="1" t="n">
+        <v>42310.7273726852</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>42310.7273726852</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -796,6 +835,21 @@
       <c r="H3" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="I3" s="1" t="n">
+        <v>42340.7273726852</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>42340.7273726852</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -822,6 +876,21 @@
       <c r="H4" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="I4" s="1" t="n">
+        <v>42371.7273726852</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>42371.7273726852</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -848,6 +917,21 @@
       <c r="H5" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="I5" s="1" t="n">
+        <v>42402.7273726852</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>42402.7273726852</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -874,6 +958,21 @@
       <c r="H6" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="I6" s="1" t="n">
+        <v>42431.7273726852</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>42431.7273726852</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -900,6 +999,21 @@
       <c r="H7" s="0" t="n">
         <v>37</v>
       </c>
+      <c r="I7" s="1" t="n">
+        <v>42462.7273726852</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>612</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>42462.7273726852</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>662</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -926,6 +1040,21 @@
       <c r="H8" s="0" t="n">
         <v>53</v>
       </c>
+      <c r="I8" s="1" t="n">
+        <v>42492.7273726852</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1088</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>42492.7273726852</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>1245</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -952,6 +1081,21 @@
       <c r="H9" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="I9" s="1" t="n">
+        <v>42523.7273726852</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1134</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>42523.7273726852</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>1332</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -978,6 +1122,21 @@
       <c r="H10" s="0" t="n">
         <v>106</v>
       </c>
+      <c r="I10" s="1" t="n">
+        <v>42553.7273726852</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1329</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>42553.7273726852</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>1617</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1004,6 +1163,21 @@
       <c r="H11" s="0" t="n">
         <v>143</v>
       </c>
+      <c r="I11" s="1" t="n">
+        <v>42584.7273726852</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1543</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>42584.7273726852</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1958</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1030,6 +1204,21 @@
       <c r="H12" s="0" t="n">
         <v>206</v>
       </c>
+      <c r="I12" s="1" t="n">
+        <v>42615.7273726852</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1657</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>42615.7273726852</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>2181</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -1056,6 +1245,21 @@
       <c r="H13" s="0" t="n">
         <v>309</v>
       </c>
+      <c r="I13" s="1" t="n">
+        <v>42645.7273726852</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1946</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>42645.7273726852</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>2693</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -1082,6 +1286,21 @@
       <c r="H14" s="0" t="n">
         <v>382</v>
       </c>
+      <c r="I14" s="1" t="n">
+        <v>42676.7273726852</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>2049</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>42676.7273726852</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>2897</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1108,6 +1327,21 @@
       <c r="H15" s="0" t="n">
         <v>447</v>
       </c>
+      <c r="I15" s="1" t="n">
+        <v>42706.7273726852</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>2129</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>42706.7273726852</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>3142</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1134,6 +1368,21 @@
       <c r="H16" s="0" t="n">
         <v>551</v>
       </c>
+      <c r="I16" s="1" t="n">
+        <v>42737.7273726852</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>2160</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>42737.7273726852</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>3279</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1160,6 +1409,21 @@
       <c r="H17" s="0" t="n">
         <v>561</v>
       </c>
+      <c r="I17" s="1" t="n">
+        <v>42768.7273726852</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>2223</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>42768.7273726852</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>3406</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1186,6 +1450,21 @@
       <c r="H18" s="0" t="n">
         <v>623</v>
       </c>
+      <c r="I18" s="1" t="n">
+        <v>42796.7273726852</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>2309</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>42796.7273726852</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>3581</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1212,6 +1491,21 @@
       <c r="H19" s="0" t="n">
         <v>627</v>
       </c>
+      <c r="I19" s="1" t="n">
+        <v>42827.7273726852</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>2310</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>42827.7273726852</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>3611</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>66</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -1238,6 +1532,21 @@
       <c r="H20" s="0" t="n">
         <v>629</v>
       </c>
+      <c r="I20" s="1" t="n">
+        <v>42857.7273726852</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>2311</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>42857.7273726852</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>3619</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1264,6 +1573,21 @@
       <c r="H21" s="0" t="n">
         <v>630</v>
       </c>
+      <c r="I21" s="1" t="n">
+        <v>42888.7273726852</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>2312</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>42888.7273726852</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>3628</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -1290,6 +1614,21 @@
       <c r="H22" s="0" t="n">
         <v>634</v>
       </c>
+      <c r="I22" s="1" t="n">
+        <v>42918.7273726852</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>2313</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>42918.7273726852</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>3636</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -1316,6 +1655,21 @@
       <c r="H23" s="0" t="n">
         <v>662</v>
       </c>
+      <c r="I23" s="1" t="n">
+        <v>42949.7273726852</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>2334</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>42949.7273726852</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>3686</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1342,6 +1696,21 @@
       <c r="H24" s="0" t="n">
         <v>695</v>
       </c>
+      <c r="I24" s="1" t="n">
+        <v>42980.7273726852</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>2390</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>42980.7273726852</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>3799</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -1368,6 +1737,21 @@
       <c r="H25" s="0" t="n">
         <v>752</v>
       </c>
+      <c r="I25" s="1" t="n">
+        <v>43010.7273726852</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>2393</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>43010.7273726852</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>3868</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1394,6 +1778,21 @@
       <c r="H26" s="0" t="n">
         <v>836</v>
       </c>
+      <c r="I26" s="1" t="n">
+        <v>43041.7273726852</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>2491</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>43041.7273726852</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>4082</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>104</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -1420,6 +1819,21 @@
       <c r="H27" s="0" t="n">
         <v>923</v>
       </c>
+      <c r="I27" s="1" t="n">
+        <v>43071.7273726852</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>2728</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>43071.7273726852</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>4482</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>118</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -1446,6 +1860,21 @@
       <c r="H28" s="0" t="n">
         <v>966</v>
       </c>
+      <c r="I28" s="1" t="n">
+        <v>43102.7273726852</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>2751</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>43102.7273726852</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>4574</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -1472,6 +1901,21 @@
       <c r="H29" s="0" t="n">
         <v>996</v>
       </c>
+      <c r="I29" s="1" t="n">
+        <v>43133.7273726852</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>2765</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>43133.7273726852</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>4640</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -1498,6 +1942,21 @@
       <c r="H30" s="0" t="n">
         <v>1069</v>
       </c>
+      <c r="I30" s="1" t="n">
+        <v>43161.7273726852</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>2894</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>43161.7273726852</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>4875</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>156</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -1524,6 +1983,21 @@
       <c r="H31" s="0" t="n">
         <v>1099</v>
       </c>
+      <c r="I31" s="1" t="n">
+        <v>43192.7273726852</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>2902</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <v>43192.7273726852</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>4937</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>163</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -1550,6 +2024,21 @@
       <c r="H32" s="0" t="n">
         <v>1159</v>
       </c>
+      <c r="I32" s="1" t="n">
+        <v>43222.7273726852</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>2903</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>43222.7273726852</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>4999</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>170</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -1576,6 +2065,21 @@
       <c r="H33" s="0" t="n">
         <v>1199</v>
       </c>
+      <c r="I33" s="1" t="n">
+        <v>43253.7273726852</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>2922</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>43253.7273726852</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>5083</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -1602,6 +2106,21 @@
       <c r="H34" s="0" t="n">
         <v>1328</v>
       </c>
+      <c r="I34" s="1" t="n">
+        <v>43283.7273726852</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>3049</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>43283.7273726852</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>5403</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>188</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -1628,6 +2147,21 @@
       <c r="H35" s="0" t="n">
         <v>1405</v>
       </c>
+      <c r="I35" s="1" t="n">
+        <v>43314.7273726852</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>3195</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>43314.7273726852</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>5701</v>
+      </c>
+      <c r="M35" s="0" t="n">
+        <v>203</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -1654,6 +2188,21 @@
       <c r="H36" s="0" t="n">
         <v>1473</v>
       </c>
+      <c r="I36" s="1" t="n">
+        <v>43345.7273726852</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>3325</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <v>43345.7273726852</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>5995</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <v>212</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -1680,6 +2229,21 @@
       <c r="H37" s="0" t="n">
         <v>1532</v>
       </c>
+      <c r="I37" s="1" t="n">
+        <v>43375.7273726852</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>3414</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>43375.7273726852</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>6183</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <v>223</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
@@ -1706,6 +2270,21 @@
       <c r="H38" s="0" t="n">
         <v>1610</v>
       </c>
+      <c r="I38" s="1" t="n">
+        <v>43406.7273726852</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>3595</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>43406.7273726852</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>6492</v>
+      </c>
+      <c r="M38" s="0" t="n">
+        <v>233</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -1732,6 +2311,21 @@
       <c r="H39" s="0" t="n">
         <v>1795</v>
       </c>
+      <c r="I39" s="1" t="n">
+        <v>43436.7273726852</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>3818</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>43436.7273726852</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>6944</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <v>244</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -1758,6 +2352,21 @@
       <c r="H40" s="0" t="n">
         <v>1897</v>
       </c>
+      <c r="I40" s="1" t="n">
+        <v>43467.7273726852</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>4037</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>43467.7273726852</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>7394</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <v>259</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -1784,6 +2393,21 @@
       <c r="H41" s="0" t="n">
         <v>1991</v>
       </c>
+      <c r="I41" s="1" t="n">
+        <v>43498.7273726852</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>4225</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <v>43498.7273726852</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>7751</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>268</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -1803,6 +2427,21 @@
       </c>
       <c r="H42" s="0" t="n">
         <v>2008</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>43526.7273726852</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>4235</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>43526.7273726852</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>7836</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>